<commit_message>
add chart for hr
</commit_message>
<xml_diff>
--- a/public/themplate-file/impor-data-karyawan.xlsx
+++ b/public/themplate-file/impor-data-karyawan.xlsx
@@ -24,13 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>aditya</t>
-  </si>
-  <si>
-    <t>manager</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>nama</t>
   </si>
@@ -48,6 +42,27 @@
   </si>
   <si>
     <t>2019-12-01</t>
+  </si>
+  <si>
+    <t>STAFF</t>
+  </si>
+  <si>
+    <t>MARKETING</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>divisi</t>
+  </si>
+  <si>
+    <t>asd</t>
+  </si>
+  <si>
+    <t>2019-12-02</t>
+  </si>
+  <si>
+    <t>sss</t>
   </si>
 </sst>
 </file>
@@ -86,9 +101,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -369,54 +385,89 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2">
+        <v>123456</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>324324</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>111111</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="E2">
+      <c r="E3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3">
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C3">
+      <formula1>"DIREKTUR UTAMA,DIREKTUR KEPATUHAN,DIREKTUR MARKETING,MANAGER,STAFF"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D3">
+      <formula1>"BOD,MARKETING,IT"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>